<commit_message>
Ajout des calculs des 3 corps
</commit_message>
<xml_diff>
--- a/ProjetGravite/Islam_Shafaatul_ProjetGravite.xlsx
+++ b/ProjetGravite/Islam_Shafaatul_ProjetGravite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\CVM\Outil de gestion\GitHub2022\ProjetGravite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03575752-E79F-4A31-B547-C80EB6C1B6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B52A124-5933-4BC9-B2CD-23BFB70B74EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FD5A80BE-EA49-45AB-B386-BF518CFC0556}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{FD5A80BE-EA49-45AB-B386-BF518CFC0556}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
   <si>
     <t>Conditions initiales de la simulation</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>Attraction</t>
+  </si>
+  <si>
+    <t>Corps 2</t>
+  </si>
+  <si>
+    <t>Corps 3</t>
   </si>
 </sst>
 </file>
@@ -199,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +215,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -225,11 +249,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -240,8 +261,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -557,36 +593,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A73D7FB-883A-44C8-9413-934BFA04663C}">
-  <dimension ref="B2:Q24"/>
+  <dimension ref="B2:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33:P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
@@ -607,64 +643,64 @@
       <c r="P4" s="6"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="4">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="5">
         <v>0.5</v>
       </c>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4" t="s">
+      <c r="N5" s="5"/>
+      <c r="O5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="P5" s="4"/>
+      <c r="P5" s="5"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="4">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="5">
         <v>0</v>
       </c>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4" t="s">
+      <c r="N6" s="5"/>
+      <c r="O6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="4"/>
+      <c r="P6" s="5"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="4">
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="5">
         <v>2</v>
       </c>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4" t="s">
+      <c r="N7" s="5"/>
+      <c r="O7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="4"/>
+      <c r="P7" s="5"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="s">
@@ -685,105 +721,105 @@
       <c r="P9" s="6"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="4">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="5">
         <v>1</v>
       </c>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4" t="s">
+      <c r="N10" s="5"/>
+      <c r="O10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P10" s="4"/>
+      <c r="P10" s="5"/>
     </row>
     <row r="11" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="3">
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="2">
         <v>0</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="2">
         <v>0</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="O11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P11" s="4"/>
+      <c r="P11" s="5"/>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="3">
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="2">
         <v>0</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12" s="2">
         <v>0</v>
       </c>
-      <c r="O12" s="4" t="s">
+      <c r="O12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="P12" s="4"/>
+      <c r="P12" s="5"/>
     </row>
     <row r="13" spans="2:17" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="3">
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="2">
         <v>0</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13" s="2">
         <v>0</v>
       </c>
-      <c r="O13" s="4" t="s">
+      <c r="O13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="P13" s="4"/>
+      <c r="P13" s="5"/>
     </row>
     <row r="14" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="4">
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="5">
         <v>2500</v>
       </c>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4" t="s">
+      <c r="N14" s="5"/>
+      <c r="O14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P14" s="4"/>
+      <c r="P14" s="5"/>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C16" s="6" t="s">
@@ -804,119 +840,486 @@
       <c r="P16" s="6"/>
     </row>
     <row r="17" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="3">
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="2">
         <v>20000</v>
       </c>
-      <c r="N18" s="3">
+      <c r="N18" s="2">
         <v>7500</v>
       </c>
-      <c r="O18" s="4" t="s">
+      <c r="O18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P18" s="4"/>
+      <c r="P18" s="5"/>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="4">
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="5">
         <v>5000</v>
       </c>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4" t="s">
+      <c r="N19" s="5"/>
+      <c r="O19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P19" s="4"/>
+      <c r="P19" s="5"/>
     </row>
     <row r="20" spans="3:16" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="O20" s="4" t="s">
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="5">
+        <v>1</v>
+      </c>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="P20" s="4"/>
+      <c r="P20" s="5"/>
     </row>
     <row r="21" spans="3:16" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O21" s="4" t="s">
+      <c r="M21" s="5">
+        <f xml:space="preserve"> (4/3)*PI()*POWER(M19,3)</f>
+        <v>523598775598.29883</v>
+      </c>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="P21" s="4"/>
+      <c r="P21" s="5"/>
     </row>
     <row r="22" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O22" s="4" t="s">
+      <c r="M22" s="5">
+        <f xml:space="preserve"> M20*M21</f>
+        <v>523598775598.29883</v>
+      </c>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="P22" s="4"/>
+      <c r="P22" s="5"/>
     </row>
     <row r="23" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="I23" s="2" t="s">
+      <c r="I23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O23" s="4" t="s">
+      <c r="M23" s="5">
+        <f xml:space="preserve"> M19*$M$7</f>
+        <v>10000</v>
+      </c>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P23" s="4"/>
+      <c r="P23" s="5"/>
     </row>
     <row r="24" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="J24" s="5" t="s">
+      <c r="J24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="4" t="s">
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="N24" s="4"/>
-      <c r="O24" s="4" t="s">
+      <c r="N24" s="5"/>
+      <c r="O24" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P24" s="4"/>
+      <c r="P24" s="5"/>
+    </row>
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+    </row>
+    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="D26" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="3">
+        <v>-20000</v>
+      </c>
+      <c r="N26" s="3">
+        <v>10000</v>
+      </c>
+      <c r="O26" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P26" s="5"/>
+    </row>
+    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="E27" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="5">
+        <v>3500</v>
+      </c>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P27" s="5"/>
+    </row>
+    <row r="28" spans="3:16" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="F28" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="6"/>
+      <c r="M28" s="5">
+        <v>1</v>
+      </c>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P28" s="5"/>
+    </row>
+    <row r="29" spans="3:16" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="G29" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M29" s="5">
+        <f xml:space="preserve"> (4/3)*PI()*POWER(M27,3)</f>
+        <v>179594380030.21649</v>
+      </c>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="P29" s="5"/>
+    </row>
+    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="H30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M30" s="5">
+        <f xml:space="preserve"> M28*M29</f>
+        <v>179594380030.21649</v>
+      </c>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="P30" s="5"/>
+    </row>
+    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="I31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M31" s="5">
+        <f xml:space="preserve"> M27*$M$7</f>
+        <v>7000</v>
+      </c>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P31" s="5"/>
+    </row>
+    <row r="32" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="J32" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="P32" s="5"/>
+    </row>
+    <row r="33" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C33" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
+      <c r="P33" s="10"/>
+    </row>
+    <row r="34" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="D34" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="3">
+        <v>-5000</v>
+      </c>
+      <c r="N34" s="3">
+        <v>-15000</v>
+      </c>
+      <c r="O34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P34" s="5"/>
+    </row>
+    <row r="35" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="E35" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="5">
+        <v>5000</v>
+      </c>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P35" s="5"/>
+    </row>
+    <row r="36" spans="3:16" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="F36" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="5">
+        <v>1</v>
+      </c>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="P36" s="5"/>
+    </row>
+    <row r="37" spans="3:16" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="G37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M37" s="5">
+        <f xml:space="preserve"> (4/3)*PI()*POWER(M35,3)</f>
+        <v>523598775598.29883</v>
+      </c>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="P37" s="5"/>
+    </row>
+    <row r="38" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="H38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M38" s="5">
+        <f xml:space="preserve"> M36*M37</f>
+        <v>523598775598.29883</v>
+      </c>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="P38" s="5"/>
+    </row>
+    <row r="39" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="I39" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M39" s="5">
+        <f xml:space="preserve"> M35*$M$7</f>
+        <v>10000</v>
+      </c>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P39" s="5"/>
+    </row>
+    <row r="40" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="J40" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="P40" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="38">
+  <mergeCells count="79">
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="O38:P38"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="O39:P39"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="O40:P40"/>
+    <mergeCell ref="F36:L36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="C33:P33"/>
+    <mergeCell ref="D34:L34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="E35:L35"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="F28:L28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="C25:P25"/>
+    <mergeCell ref="F20:L20"/>
+    <mergeCell ref="D26:L26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="E27:L27"/>
+    <mergeCell ref="M27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="C4:P4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="M5:N5"/>
+    <mergeCell ref="D5:L5"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="E6:L6"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="M7:N7"/>
+    <mergeCell ref="F7:L7"/>
+    <mergeCell ref="C9:P9"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="D10:L10"/>
+    <mergeCell ref="E11:L11"/>
+    <mergeCell ref="F12:L12"/>
+    <mergeCell ref="G13:L13"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="C16:P16"/>
+    <mergeCell ref="C17:P17"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="D18:L18"/>
+    <mergeCell ref="O19:P19"/>
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="E19:L19"/>
     <mergeCell ref="J24:L24"/>
     <mergeCell ref="O20:P20"/>
     <mergeCell ref="O21:P21"/>
@@ -924,37 +1327,10 @@
     <mergeCell ref="O23:P23"/>
     <mergeCell ref="O24:P24"/>
     <mergeCell ref="M24:N24"/>
-    <mergeCell ref="C16:P16"/>
-    <mergeCell ref="C17:P17"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="D18:L18"/>
-    <mergeCell ref="O19:P19"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="E19:L19"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="D10:L10"/>
-    <mergeCell ref="E11:L11"/>
-    <mergeCell ref="F12:L12"/>
-    <mergeCell ref="G13:L13"/>
-    <mergeCell ref="H14:L14"/>
-    <mergeCell ref="C9:P9"/>
-    <mergeCell ref="M10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="E6:L6"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="M7:N7"/>
-    <mergeCell ref="F7:L7"/>
-    <mergeCell ref="B2:Q2"/>
-    <mergeCell ref="C4:P4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="M5:N5"/>
-    <mergeCell ref="D5:L5"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M22:N22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>